<commit_message>
changes to the observations to add distance travelled
</commit_message>
<xml_diff>
--- a/examples/tmp_dir/my_a_matrix.xlsx
+++ b/examples/tmp_dir/my_a_matrix.xlsx
@@ -8,30 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao\Desktop\projects\nested\pymdp\examples\tmp_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A01CC2-D7C1-4CD0-8E7C-23180B2D5316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608F34D-759B-4512-A788-1F02AD13CC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>current_location</t>
   </si>
@@ -139,6 +128,27 @@
   </si>
   <si>
     <t>distance25</t>
+  </si>
+  <si>
+    <t>distance_travelled</t>
+  </si>
+  <si>
+    <t>distancet0</t>
+  </si>
+  <si>
+    <t>distancet5</t>
+  </si>
+  <si>
+    <t>distancet10</t>
+  </si>
+  <si>
+    <t>distancet15</t>
+  </si>
+  <si>
+    <t>distancet20</t>
+  </si>
+  <si>
+    <t>distance25t</t>
   </si>
 </sst>
 </file>
@@ -507,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN17"/>
+  <dimension ref="A1:BN23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AV16" sqref="AV16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,28 +826,28 @@
         <v>21</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -1038,28 +1048,28 @@
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -1260,28 +1270,28 @@
         <v>0</v>
       </c>
       <c r="S6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="1">
         <v>0</v>
@@ -1482,28 +1492,28 @@
         <v>0</v>
       </c>
       <c r="AA7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="1">
         <v>0</v>
@@ -1704,28 +1714,28 @@
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ8" s="1">
         <v>0</v>
@@ -1926,28 +1936,28 @@
         <v>0</v>
       </c>
       <c r="AQ9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY9" s="1">
         <v>0</v>
@@ -2148,28 +2158,28 @@
         <v>0</v>
       </c>
       <c r="AY10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG10" s="1">
         <v>0</v>
@@ -2370,28 +2380,28 @@
         <v>0</v>
       </c>
       <c r="BG11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:66" ht="30" x14ac:dyDescent="0.25">
@@ -2402,7 +2412,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -2429,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -2456,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="U12" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
@@ -2483,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="AD12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="1">
         <v>0</v>
@@ -2510,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="AM12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="1">
         <v>0</v>
@@ -2537,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="AV12" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AW12" s="1">
         <v>0</v>
@@ -2564,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="BE12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF12" s="1">
         <v>0</v>
@@ -2591,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="BN12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:66" ht="30" x14ac:dyDescent="0.25">
@@ -2603,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -2624,13 +2634,13 @@
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
@@ -2651,19 +2661,19 @@
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U13" s="1">
         <v>0</v>
       </c>
       <c r="V13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <v>0</v>
       </c>
       <c r="X13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="1">
         <v>0</v>
@@ -2678,13 +2688,13 @@
         <v>0</v>
       </c>
       <c r="AC13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="1">
         <v>0</v>
       </c>
       <c r="AE13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
@@ -2705,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM13" s="1">
         <v>0</v>
@@ -2732,13 +2742,13 @@
         <v>0</v>
       </c>
       <c r="AU13" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AV13" s="1">
         <v>0</v>
       </c>
       <c r="AW13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX13" s="1">
         <v>0</v>
@@ -2759,13 +2769,13 @@
         <v>0</v>
       </c>
       <c r="BD13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="1">
         <v>0</v>
       </c>
       <c r="BF13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG13" s="1">
         <v>0</v>
@@ -2786,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN13" s="1">
         <v>0</v>
@@ -2804,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2831,13 +2841,13 @@
         <v>0</v>
       </c>
       <c r="N14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
       </c>
       <c r="P14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="1">
         <v>0</v>
@@ -2846,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="1">
         <v>0</v>
@@ -2858,13 +2868,13 @@
         <v>0</v>
       </c>
       <c r="W14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="1">
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="1">
         <v>0</v>
@@ -2873,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="1">
         <v>0</v>
@@ -2885,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="1">
         <v>0</v>
@@ -2900,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="AK14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="1">
         <v>0</v>
@@ -2921,13 +2931,13 @@
         <v>0</v>
       </c>
       <c r="AR14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AS14" s="1">
         <v>0</v>
       </c>
       <c r="AT14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AU14" s="1">
         <v>0</v>
@@ -2939,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="AX14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY14" s="1">
         <v>0</v>
@@ -2948,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="BA14" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BB14" s="1">
         <v>0</v>
@@ -2981,7 +2991,7 @@
         <v>0</v>
       </c>
       <c r="BL14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM14" s="1">
         <v>0</v>
@@ -3005,13 +3015,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -3032,13 +3042,13 @@
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
@@ -3065,10 +3075,10 @@
         <v>0</v>
       </c>
       <c r="Z15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="1">
         <v>0</v>
@@ -3086,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="AG15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="1">
         <v>0</v>
@@ -3095,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK15" s="1">
         <v>0</v>
@@ -3107,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="AN15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO15" s="1">
         <v>0</v>
@@ -3116,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="AQ15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR15" s="1">
         <v>0</v>
@@ -3128,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="AU15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AV15" s="1">
         <v>0</v>
@@ -3143,13 +3153,13 @@
         <v>0</v>
       </c>
       <c r="AZ15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BA15" s="1">
         <v>0</v>
       </c>
       <c r="BB15" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BC15" s="1">
         <v>0</v>
@@ -3170,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="BI15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ15" s="1">
         <v>0</v>
@@ -3206,13 +3216,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
@@ -3239,7 +3249,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="1">
         <v>0</v>
@@ -3248,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="U16" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
@@ -3260,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
@@ -3287,10 +3297,10 @@
         <v>0</v>
       </c>
       <c r="AH16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="1">
         <v>0</v>
@@ -3308,7 +3318,7 @@
         <v>0</v>
       </c>
       <c r="AO16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP16" s="1">
         <v>0</v>
@@ -3317,19 +3327,19 @@
         <v>0</v>
       </c>
       <c r="AR16" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AS16" s="1">
         <v>0</v>
       </c>
       <c r="AT16" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AU16" s="1">
         <v>0</v>
       </c>
       <c r="AV16" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AW16" s="1">
         <v>0</v>
@@ -3338,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="AY16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ16" s="1">
         <v>0</v>
@@ -3350,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="BC16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD16" s="1">
         <v>0</v>
@@ -3365,13 +3375,13 @@
         <v>0</v>
       </c>
       <c r="BH16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI16" s="1">
         <v>0</v>
       </c>
       <c r="BJ16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK16" s="1">
         <v>0</v>
@@ -3413,7 +3423,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
@@ -3422,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="M17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O17" s="1">
         <v>0</v>
@@ -3434,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
@@ -3443,19 +3453,19 @@
         <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="U17" s="1">
         <v>0</v>
       </c>
       <c r="V17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W17" s="1">
         <v>0</v>
       </c>
       <c r="X17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="1">
         <v>0</v>
@@ -3464,13 +3474,13 @@
         <v>0</v>
       </c>
       <c r="AA17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
       </c>
       <c r="AC17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="1">
         <v>0</v>
@@ -3482,7 +3492,7 @@
         <v>0</v>
       </c>
       <c r="AG17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="1">
         <v>0</v>
@@ -3509,7 +3519,7 @@
         <v>0</v>
       </c>
       <c r="AP17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ17" s="1">
         <v>0</v>
@@ -3518,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="AS17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT17" s="1">
         <v>0</v>
@@ -3539,13 +3549,13 @@
         <v>0</v>
       </c>
       <c r="AZ17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BA17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BB17" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="1">
         <v>0</v>
@@ -3560,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH17" s="1">
         <v>0</v>
@@ -3572,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="BK17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL17" s="1">
         <v>0</v>
@@ -3581,11 +3591,1202 @@
         <v>0</v>
       </c>
       <c r="BN17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:66" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BK23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN23" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A18:A23"/>
     <mergeCell ref="AQ1:AX1"/>
     <mergeCell ref="AY1:BF1"/>
     <mergeCell ref="BG1:BN1"/>

</xml_diff>